<commit_message>
formated tables the lyx way before pasting into lyx
</commit_message>
<xml_diff>
--- a/midline/consumption_treatment/papers/Tables_for_lyx.xlsx
+++ b/midline/consumption_treatment/papers/Tables_for_lyx.xlsx
@@ -5,17 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LNabwire\OneDrive - CGIAR\L.Nabwire\git\Maize_Uganda\mippi_UG\midline\consumption_treatment\papers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgiar-my.sharepoint.com/personal/l_nabwire_cgiar_org/Documents/L.Nabwire/git/Maize_Uganda/mippi_UG/midline/consumption_treatment/papers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CFB958-9B62-49CF-95B9-FB691957B4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{69CFB958-9B62-49CF-95B9-FB691957B4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C1F2BE-F558-4E25-AA05-BD549EA3131D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
     <sheet name="Perceptions_before" sheetId="2" r:id="rId2"/>
     <sheet name="Perceptions_after" sheetId="4" r:id="rId3"/>
+    <sheet name="Perceptions_before_%" sheetId="5" r:id="rId4"/>
+    <sheet name="Perceptions_after_%" sheetId="6" r:id="rId5"/>
+    <sheet name="Combined" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="65">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -355,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -449,6 +452,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1501,7 +1507,7 @@
   <dimension ref="A1:AA28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2697,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46FBA75-DDA1-4C8C-800D-9B8D4AB3C152}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3622,4 +3628,2631 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE2A4A4-5CDB-4699-B84E-57587A78BBE7}">
+  <dimension ref="A1:AA28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.90625" customWidth="1"/>
+    <col min="2" max="2" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="1.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A2" s="17"/>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="20"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="16"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="18">
+        <v>78</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16">
+        <v>60.53</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="16">
+        <v>39.47</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="16">
+        <v>21.07</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="16"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="16">
+        <v>59.08</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="16">
+        <v>40.92</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="16">
+        <v>18.16</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="16"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="21">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="16">
+        <v>61.72</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16">
+        <v>38.28</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="16">
+        <v>23.43</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="16"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="18">
+        <v>78</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="16">
+        <v>85.18</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16">
+        <v>14.82</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="16">
+        <v>70.349999999999994</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="16"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18">
+        <v>78</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="16">
+        <v>28.06</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="16">
+        <v>71.94</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="16">
+        <v>-43.88</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="19">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="16"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="18">
+        <v>78</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="16">
+        <v>68.28</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="16">
+        <v>31.72</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="16">
+        <v>36.56</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="19">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="16"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18">
+        <v>78</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>74.87</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="16">
+        <v>25.13</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="16">
+        <v>49.74</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="16"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18">
+        <v>78</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="16">
+        <v>58.71</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="16">
+        <v>41.29</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="16">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0.08</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="16"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18">
+        <v>78</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="16">
+        <v>34.409999999999997</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="16">
+        <v>65.59</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="16">
+        <v>-31.18</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="19">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" s="16"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="18">
+        <v>78</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="16">
+        <v>79.25</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="16">
+        <v>20.75</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="16">
+        <v>58.49</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="20"/>
+      <c r="N19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="20"/>
+      <c r="N20" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="36">
+        <v>40.92</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="36">
+        <v>38.28</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="36">
+        <v>0.64</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="36">
+        <v>59.08</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="36">
+        <v>61.72</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="36">
+        <v>0.64</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="36">
+        <v>13.83</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="36">
+        <v>15.61</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="36">
+        <v>0.78</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="36">
+        <v>86.17</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="36">
+        <v>84.39</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="36">
+        <v>0.78</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="36">
+        <v>75.25</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="36">
+        <v>69.25</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="36">
+        <v>0.4</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="36">
+        <v>24.75</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="36">
+        <v>30.75</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="36">
+        <v>0.4</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="36">
+        <v>27</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="36">
+        <v>35.54</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="36">
+        <v>0.34</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="36">
+        <v>73</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="36">
+        <v>64.459999999999994</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="36">
+        <v>0.34</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="36">
+        <v>24.17</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="36">
+        <v>25.82</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="36">
+        <v>0.84</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="36">
+        <v>75.83</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="36">
+        <v>74.180000000000007</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="36">
+        <v>0.84</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="36">
+        <v>46.68</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="36">
+        <v>37.03</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="36">
+        <v>53.32</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="36">
+        <v>62.97</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="36">
+        <v>67.73</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="36">
+        <v>63.85</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="36">
+        <v>0.64</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="36">
+        <v>32.270000000000003</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="36">
+        <v>36.15</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="36">
+        <v>0.64</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="36">
+        <v>21.07</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="36">
+        <v>20.51</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="36">
+        <v>0.93</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="36">
+        <v>78.930000000000007</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="36">
+        <v>79.489999999999995</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="36">
+        <v>0.93</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="V4:Z4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E250B4F-61EA-4751-96DF-FD469D157218}">
+  <dimension ref="A1:N28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="1.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="25"/>
+      <c r="J3" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="30"/>
+      <c r="J4" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="26">
+        <v>78</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="36">
+        <v>12.19</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="36">
+        <v>-12.19</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="36">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="27">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="36">
+        <v>12.75</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="36">
+        <v>-12.75</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="36">
+        <v>0.01</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="32">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="36">
+        <v>11.73</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="36">
+        <v>-11.73</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="36">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="26">
+        <v>78</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="36">
+        <v>10.88</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="36">
+        <v>-10.88</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="36">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="26">
+        <v>78</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="36">
+        <v>26.24</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="36">
+        <v>-26.24</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="36">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="26">
+        <v>78</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="36">
+        <v>6.87</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="36">
+        <v>-6.87</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="36">
+        <v>0.17</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="26">
+        <v>78</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="36">
+        <v>-7.11</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="36">
+        <v>7.11</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="36">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="26">
+        <v>78</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="36">
+        <v>7.19</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="36">
+        <v>-7.19</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="36">
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="26">
+        <v>78</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="36">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="36">
+        <v>-35.299999999999997</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="36">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="26">
+        <v>78</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="36">
+        <v>1.78</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="36">
+        <v>-1.78</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="36">
+        <v>0.71</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="35"/>
+    </row>
+    <row r="18" spans="1:14" ht="26" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="28"/>
+      <c r="N19" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="K20" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="M20" s="28"/>
+      <c r="N20" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="36">
+        <v>-12.75</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="36">
+        <v>-11.73</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="36">
+        <v>0.86</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="36">
+        <v>12.75</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K21" s="36">
+        <v>11.73</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M21" s="36">
+        <v>0.86</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="36">
+        <v>-7.71</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="36">
+        <v>-13.39</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="36">
+        <v>0.36</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="36">
+        <v>7.71</v>
+      </c>
+      <c r="J22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="36">
+        <v>13.39</v>
+      </c>
+      <c r="L22" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="36">
+        <v>0.36</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="36">
+        <v>-28.37</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="36">
+        <v>-24.51</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="36">
+        <v>0.67</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="36">
+        <v>28.37</v>
+      </c>
+      <c r="J23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K23" s="36">
+        <v>24.51</v>
+      </c>
+      <c r="L23" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" s="36">
+        <v>0.67</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="36">
+        <v>-4.91</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="36">
+        <v>-8.41</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="36">
+        <v>0.73</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="36">
+        <v>4.91</v>
+      </c>
+      <c r="J24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="36">
+        <v>8.41</v>
+      </c>
+      <c r="L24" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M24" s="36">
+        <v>0.73</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="36">
+        <v>15</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="36">
+        <v>1.42</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="36">
+        <v>-15</v>
+      </c>
+      <c r="J25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K25" s="36">
+        <v>-1.42</v>
+      </c>
+      <c r="L25" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="36">
+        <v>-12.65</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="36">
+        <v>-3</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="36">
+        <v>0.44</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="36">
+        <v>12.65</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="36">
+        <v>3</v>
+      </c>
+      <c r="L26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M26" s="36">
+        <v>0.44</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="36">
+        <v>-33.24</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="36">
+        <v>-36.979999999999997</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="36">
+        <v>0.71</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="36">
+        <v>33.24</v>
+      </c>
+      <c r="J27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="36">
+        <v>36.979999999999997</v>
+      </c>
+      <c r="L27" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M27" s="36">
+        <v>0.71</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="36">
+        <v>-8.76</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="36">
+        <v>3.73</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="36">
+        <v>0.21</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="36">
+        <v>8.76</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="36">
+        <v>-3.73</v>
+      </c>
+      <c r="L28" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="M28" s="36">
+        <v>0.21</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="I17:M17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7EC6BED-65F7-45D9-86B6-CDEED3F9CC72}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="41.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="17"/>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="18">
+        <v>78</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16">
+        <v>60.53</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="16">
+        <v>39.47</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="16">
+        <v>21.07</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="19">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="16">
+        <v>35</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="16">
+        <v>59.08</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="16">
+        <v>40.92</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="16">
+        <v>18.16</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="21">
+        <v>43</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="16">
+        <v>61.72</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="16">
+        <v>38.28</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="16">
+        <v>23.43</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="18">
+        <v>78</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="16">
+        <v>85.18</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="16">
+        <v>14.82</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="16">
+        <v>70.349999999999994</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="19">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18">
+        <v>78</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="16">
+        <v>28.06</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="16">
+        <v>71.94</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="16">
+        <v>-43.88</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="19">
+        <v>0</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="18">
+        <v>78</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="16">
+        <v>68.28</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="16">
+        <v>31.72</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="16">
+        <v>36.56</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="19">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18">
+        <v>78</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="16">
+        <v>74.87</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="16">
+        <v>25.13</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="16">
+        <v>49.74</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="18">
+        <v>78</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="16">
+        <v>58.71</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="16">
+        <v>41.29</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="16">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="19">
+        <v>0.08</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="18">
+        <v>78</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="16">
+        <v>34.409999999999997</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="16">
+        <v>65.59</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="16">
+        <v>-31.18</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="19">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="18">
+        <v>78</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="16">
+        <v>79.25</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="16">
+        <v>20.75</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="16">
+        <v>58.49</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="19">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>